<commit_message>
Updaing with Multicolor Buttoms
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374D2D19-C772-4B87-99DE-5C117559B90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0866E6-BEF0-4856-A302-547BE018667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="556">
   <si>
     <t>Name</t>
   </si>
@@ -1627,18 +1627,6 @@
     <t>btnS</t>
   </si>
   <si>
-    <t>Width: 300px</t>
-  </si>
-  <si>
-    <t>Width: 120px</t>
-  </si>
-  <si>
-    <t>Width: 200px</t>
-  </si>
-  <si>
-    <t>Width: 40px</t>
-  </si>
-  <si>
     <t>Image Container</t>
   </si>
   <si>
@@ -1658,6 +1646,66 @@
   </si>
   <si>
     <t xml:space="preserve">Small Img of 70x70, Name, Position, Description | Color : red, green, yellow, blue, gray </t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>For Showcase Galary</t>
+  </si>
+  <si>
+    <t>CardTextSliding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image Full card cover, Image name, category, Small Description, button, product ID | Orientation : both </t>
+  </si>
+  <si>
+    <t>bgColorBlue</t>
+  </si>
+  <si>
+    <t>bgColorYellow</t>
+  </si>
+  <si>
+    <t>bgColorRed</t>
+  </si>
+  <si>
+    <t>bgColorCyan</t>
+  </si>
+  <si>
+    <t>bgColorGreen</t>
+  </si>
+  <si>
+    <t>bgColorSkyBlue</t>
+  </si>
+  <si>
+    <t>bgColorGray1</t>
+  </si>
+  <si>
+    <t>bgColorGray2</t>
+  </si>
+  <si>
+    <t>bgColorGray3</t>
+  </si>
+  <si>
+    <t>bgColorGray4</t>
+  </si>
+  <si>
+    <t>bgColorGray5</t>
+  </si>
+  <si>
+    <t>bgCFolorGray6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width: 120px | Color : red, green, yellow, blue, gray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width: 200px | Color : red, green, yellow, blue, gray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width: 300px | Color : red, green, yellow, blue, gray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width: 40px | Color : red, green, yellow, blue, gray </t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2254,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2301,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -2343,7 +2391,7 @@
         <v>110</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>530</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2370,7 +2418,7 @@
         <v>526</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>531</v>
+        <v>553</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2397,7 +2445,7 @@
         <v>527</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>529</v>
+        <v>554</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2424,7 +2472,7 @@
         <v>528</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>532</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,16 +2490,16 @@
         <v>16</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2469,13 +2517,16 @@
         <v>16</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>538</v>
+        <v>533</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>534</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2488,6 +2539,21 @@
       <c r="C11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>009</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6133,10 +6199,10 @@
   <dimension ref="A1:H339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomRight" activeCell="A58" sqref="A58:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7638,151 +7704,331 @@
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="10">
         <v>56</v>
       </c>
-      <c r="C58" s="5" t="str">
+      <c r="C58" s="11" t="str">
         <f t="shared" si="0"/>
         <v>038</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="D58" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="10">
         <v>57</v>
       </c>
-      <c r="C59" s="5" t="str">
+      <c r="C59" s="11" t="str">
         <f t="shared" si="0"/>
         <v>039</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="D59" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="10">
         <v>58</v>
       </c>
-      <c r="C60" s="5" t="str">
+      <c r="C60" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03A</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="D60" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="10">
         <v>59</v>
       </c>
-      <c r="C61" s="5" t="str">
+      <c r="C61" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03B</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="D61" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="10">
         <v>60</v>
       </c>
-      <c r="C62" s="5" t="str">
+      <c r="C62" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03C</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="D62" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="10">
         <v>61</v>
       </c>
-      <c r="C63" s="5" t="str">
+      <c r="C63" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03D</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="D63" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="10">
         <v>62</v>
       </c>
-      <c r="C64" s="5" t="str">
+      <c r="C64" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03E</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="D64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="10">
         <v>63</v>
       </c>
-      <c r="C65" s="5" t="str">
+      <c r="C65" s="11" t="str">
         <f t="shared" si="0"/>
         <v>03F</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="D65" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="10">
         <v>64</v>
       </c>
-      <c r="C66" s="5" t="str">
+      <c r="C66" s="11" t="str">
         <f t="shared" si="0"/>
         <v>040</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="D66" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="10">
         <v>65</v>
       </c>
-      <c r="C67" s="5" t="str">
+      <c r="C67" s="11" t="str">
         <f t="shared" si="0"/>
         <v>041</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="D67" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="10">
         <v>66</v>
       </c>
-      <c r="C68" s="5" t="str">
+      <c r="C68" s="11" t="str">
         <f t="shared" si="0"/>
         <v>042</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="D68" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="10">
         <v>67</v>
       </c>
-      <c r="C69" s="5" t="str">
+      <c r="C69" s="11" t="str">
         <f t="shared" si="0"/>
         <v>043</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>198</v>
       </c>
@@ -7794,7 +8040,7 @@
         <v>044</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
@@ -7806,7 +8052,7 @@
         <v>045</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>200</v>
       </c>
@@ -7818,7 +8064,7 @@
         <v>046</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>201</v>
       </c>
@@ -7830,7 +8076,7 @@
         <v>047</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>202</v>
       </c>
@@ -7842,7 +8088,7 @@
         <v>048</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>203</v>
       </c>
@@ -7854,7 +8100,7 @@
         <v>049</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>204</v>
       </c>
@@ -7866,7 +8112,7 @@
         <v>04A</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>205</v>
       </c>
@@ -7878,7 +8124,7 @@
         <v>04B</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -7890,7 +8136,7 @@
         <v>04C</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>207</v>
       </c>
@@ -7902,7 +8148,7 @@
         <v>04D</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>208</v>
       </c>

</xml_diff>

<commit_message>
Final Version of Header
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6F70B9-3522-487E-AD61-480D50345D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E704657-5077-492B-9421-32C2704894FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
   <sheets>
     <sheet name="Used Code" sheetId="3" r:id="rId1"/>
-    <sheet name="util" sheetId="4" r:id="rId2"/>
-    <sheet name="CSS" sheetId="5" r:id="rId3"/>
+    <sheet name="JSX1" sheetId="4" r:id="rId2"/>
+    <sheet name="CSS1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="585">
   <si>
     <t>Name</t>
   </si>
@@ -1757,6 +1757,42 @@
   </si>
   <si>
     <t>{authorName, date, imgPath, desc, productID = null, orientation = "H" }</t>
+  </si>
+  <si>
+    <t>generalPublic</t>
+  </si>
+  <si>
+    <t>helper</t>
+  </si>
+  <si>
+    <t>GetDimension</t>
+  </si>
+  <si>
+    <t>To get the Height &amp; width of the window whenever the size changes</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>crossIcon</t>
+  </si>
+  <si>
+    <t>linesicon</t>
+  </si>
+  <si>
+    <t>Icon in cross Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two lines that is used for Show hide </t>
+  </si>
+  <si>
+    <t>jsx</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Use for header</t>
   </si>
 </sst>
 </file>
@@ -2302,10 +2338,10 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,55 +2785,103 @@
         <v>559</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="10">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="str">
+      <c r="C16" s="11" t="str">
         <f t="shared" si="0"/>
         <v>00E</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="D16" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="10">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="11" t="str">
         <f t="shared" si="0"/>
         <v>00F</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="D17" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="10">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="str">
+      <c r="C18" s="11" t="str">
         <f t="shared" si="0"/>
         <v>010</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="D18" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="10">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="str">
+      <c r="C19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>011</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>130</v>
       </c>
@@ -2809,7 +2893,7 @@
         <v>012</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>131</v>
       </c>
@@ -2821,7 +2905,7 @@
         <v>013</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>132</v>
       </c>
@@ -2833,7 +2917,7 @@
         <v>014</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>133</v>
       </c>
@@ -2845,7 +2929,7 @@
         <v>015</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
@@ -2857,7 +2941,7 @@
         <v>016</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>135</v>
       </c>
@@ -2869,7 +2953,7 @@
         <v>017</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>136</v>
       </c>
@@ -2881,7 +2965,7 @@
         <v>018</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>137</v>
       </c>
@@ -2893,7 +2977,7 @@
         <v>019</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>138</v>
       </c>
@@ -2905,7 +2989,7 @@
         <v>01A</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>139</v>
       </c>
@@ -2917,7 +3001,7 @@
         <v>01B</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>140</v>
       </c>
@@ -2929,7 +3013,7 @@
         <v>01C</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>141</v>
       </c>
@@ -2941,7 +3025,7 @@
         <v>01D</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>142</v>
       </c>
@@ -6327,7 +6411,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A17:A23 D17:H23">
+  <conditionalFormatting sqref="A17:A23 D19:H23 E17:H18">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Progress on GridImage Compponent
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE1853C-E914-4998-A04D-242010636643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B67CD-D7EC-441F-981A-3E0C25B2279E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="589">
   <si>
     <t>Name</t>
   </si>
@@ -1895,6 +1895,33 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (Single Digit)</t>
+    </r>
+  </si>
+  <si>
+    <t>ResolveImageGridID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">getCellFromRowId, getCellFromColId, getNumbersOnlyFromList, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next LT Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>resolveImageGridID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next LT Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
 </sst>
@@ -2444,7 +2471,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,7 +3035,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>131</v>
       </c>
@@ -3019,6 +3046,18 @@
         <f t="shared" si="0"/>
         <v>013</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3030,6 +3069,9 @@
       <c r="C22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>014</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding Logo Files & Images
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF3778F-8861-4D4E-887E-F0962B5A0113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BD414-AD3B-4E2B-AE22-7ACC86EE726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="596">
   <si>
     <t>Name</t>
   </si>
@@ -1933,6 +1933,18 @@
   </si>
   <si>
     <t>Function that resolve IDs based on the list value : number=cellNo, R1=rowNo, C1=columnNo</t>
+  </si>
+  <si>
+    <t>creative Logo</t>
+  </si>
+  <si>
+    <t>{ width, type = 0}</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>type = 0 : written in single row, type=1:  written in two row, else: two rows with logo</t>
   </si>
 </sst>
 </file>
@@ -2478,10 +2490,10 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,19 +3090,34 @@
         <v>591</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="10">
         <v>20</v>
       </c>
-      <c r="C22" s="5" t="str">
+      <c r="C22" s="11" t="str">
         <f t="shared" si="0"/>
         <v>014</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>573</v>
+      <c r="D22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6587,7 +6614,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E17:H18 A17:A23 D22:H23 D21:G21 D19:H20">
+  <conditionalFormatting sqref="E17:H18 A17:A23 D19:H20 D21:G21 D22:H23">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update, Add India map
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB3BA91-BB01-4720-937B-06E6E29A7FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966E19A5-4ADE-4926-A920-5E27F228A01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -2574,7 +2574,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,144 +3315,144 @@
         <v>608</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="10">
         <v>25</v>
       </c>
-      <c r="C27" s="5" t="str">
+      <c r="C27" s="11" t="str">
         <f t="shared" si="0"/>
         <v>019</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="9" t="s">
         <v>609</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="9" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="10">
         <v>26</v>
       </c>
-      <c r="C28" s="5" t="str">
+      <c r="C28" s="11" t="str">
         <f t="shared" si="0"/>
         <v>01A</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="9" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="10">
         <v>27</v>
       </c>
-      <c r="C29" s="5" t="str">
+      <c r="C29" s="11" t="str">
         <f t="shared" si="0"/>
         <v>01B</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="9" t="s">
         <v>603</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="9" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="10">
         <v>28</v>
       </c>
-      <c r="C30" s="5" t="str">
+      <c r="C30" s="11" t="str">
         <f t="shared" ref="C30:C67" si="1">IF(B30&lt;&gt;"", DEC2HEX(B30, 3), "")</f>
         <v>01C</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="9" t="s">
         <v>603</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="9" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="10">
         <v>29</v>
       </c>
-      <c r="C31" s="5" t="str">
+      <c r="C31" s="11" t="str">
         <f t="shared" si="1"/>
         <v>01D</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="9" t="s">
         <v>603</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="9" t="s">
         <v>622</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update OnloadScreen, add LogoWritten
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966E19A5-4ADE-4926-A920-5E27F228A01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E6E5F3-DF62-45E6-923A-4D4FCF39114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="627">
   <si>
     <t>Name</t>
   </si>
@@ -2026,6 +2026,18 @@
   </si>
   <si>
     <t>For Searching through Data</t>
+  </si>
+  <si>
+    <t>Written Logo</t>
+  </si>
+  <si>
+    <t>LogoWritten</t>
+  </si>
+  <si>
+    <t>Logo written by self</t>
+  </si>
+  <si>
+    <t>{size='1em'}</t>
   </si>
 </sst>
 </file>
@@ -2571,10 +2583,10 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3456,16 +3468,34 @@
         <v>622</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="10">
         <v>30</v>
       </c>
-      <c r="C32" s="5" t="str">
+      <c r="C32" s="11" t="str">
         <f t="shared" si="1"/>
         <v>01E</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update, Adding Images for Place Where I serve
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D2EBD6-523F-421B-BBD9-0C432C6C272D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2C8C57-7B8E-47E5-863F-F2932B2824E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9705" yWindow="0" windowWidth="19200" windowHeight="16305" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -1748,9 +1748,6 @@
   </si>
   <si>
     <t>{ imgPath, name, title = null, desc, borderCol = "cyan", }</t>
-  </si>
-  <si>
-    <t>{ imgPath, productName, desc, btnLink = "#", productID = null, color = "blue", orientation = "S", }</t>
   </si>
   <si>
     <t>Parameters</t>
@@ -2068,6 +2065,9 @@
   </si>
   <si>
     <t>Side tabs : it have contents and onclick of that we get tranfered to different  location</t>
+  </si>
+  <si>
+    <t>{ imgPath, productName, desc, btnLink = "#", productID = null, color = "cyan", orientation = "S", }</t>
   </si>
 </sst>
 </file>
@@ -2613,10 +2613,10 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2943,7 +2943,7 @@
         <v>538</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>570</v>
+        <v>636</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>556</v>
@@ -2973,7 +2973,7 @@
         <v>555</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>557</v>
@@ -3072,16 +3072,16 @@
         <v>00E</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>574</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>575</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3096,16 +3096,16 @@
         <v>00F</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>578</v>
-      </c>
       <c r="I17" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3120,16 +3120,16 @@
         <v>010</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3144,16 +3144,16 @@
         <v>011</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>583</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3168,19 +3168,19 @@
         <v>012</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G20" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>585</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3195,22 +3195,22 @@
         <v>013</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>574</v>
-      </c>
       <c r="F21" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>587</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>588</v>
-      </c>
       <c r="H21" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>590</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3228,19 +3228,19 @@
         <v>16</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>594</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3258,16 +3258,16 @@
         <v>16</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>598</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3282,22 +3282,22 @@
         <v>016</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E24" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>600</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>601</v>
-      </c>
       <c r="G24" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H24" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I24" s="9" t="s">
         <v>603</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3312,22 +3312,22 @@
         <v>017</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F25" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>603</v>
-      </c>
       <c r="I25" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3342,19 +3342,19 @@
         <v>018</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>606</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>607</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>607</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3369,13 +3369,13 @@
         <v>019</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>609</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="I27" s="9" t="s">
         <v>610</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3390,22 +3390,22 @@
         <v>01A</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E28" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>614</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3420,22 +3420,22 @@
         <v>01B</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F29" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I29" s="9" t="s">
         <v>616</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3450,22 +3450,22 @@
         <v>01C</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F30" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I30" s="9" t="s">
         <v>618</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3480,22 +3480,22 @@
         <v>01D</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F31" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>621</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3510,22 +3510,22 @@
         <v>01E</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3540,22 +3540,22 @@
         <v>01F</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F33" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>626</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3570,22 +3570,22 @@
         <v>020</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="H34" s="9" t="s">
         <v>629</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>629</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="I34" s="9" t="s">
         <v>630</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3600,52 +3600,52 @@
         <v>021</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F35" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I35" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>632</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="10">
         <v>34</v>
       </c>
-      <c r="C36" s="5" t="str">
+      <c r="C36" s="11" t="str">
         <f t="shared" si="1"/>
         <v>022</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="F36" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="9" t="s">
         <v>635</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -7033,7 +7033,7 @@
         <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update, Add AllSector, ServiceIntro
</commit_message>
<xml_diff>
--- a/Design Requirement/Codes iRt Creative.xlsx
+++ b/Design Requirement/Codes iRt Creative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\Design Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2C8C57-7B8E-47E5-863F-F2932B2824E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E1ADC5-780C-4D74-B1C8-4DA421FFE91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9705" yWindow="0" windowWidth="19200" windowHeight="16305" activeTab="1" xr2:uid="{F32AC0A1-ED0B-4BE2-B833-AC1095930237}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="648">
   <si>
     <t>Name</t>
   </si>
@@ -2069,6 +2069,39 @@
   <si>
     <t>{ imgPath, productName, desc, btnLink = "#", productID = null, color = "cyan", orientation = "S", }</t>
   </si>
+  <si>
+    <t>OnLoadScreen</t>
+  </si>
+  <si>
+    <t>We can say this the Home page for Service Tab</t>
+  </si>
+  <si>
+    <t>WhereWeServe</t>
+  </si>
+  <si>
+    <t>DataWeServe</t>
+  </si>
+  <si>
+    <t>ServeData</t>
+  </si>
+  <si>
+    <t>has all the places where we can work like Houses, Offices, etc</t>
+  </si>
+  <si>
+    <t>our json data that has all the places where we can work has category, spces, images</t>
+  </si>
+  <si>
+    <t>OurStructure</t>
+  </si>
+  <si>
+    <t>Our json Data: Mapped, Dicision, Departments, Services, Sectors</t>
+  </si>
+  <si>
+    <t>ServiceIntro</t>
+  </si>
+  <si>
+    <t>Service Introductory Lines</t>
+  </si>
 </sst>
 </file>
 
@@ -2156,7 +2189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2190,6 +2223,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2613,10 +2655,10 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,64 +3690,151 @@
         <v>635</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="15">
         <v>35</v>
       </c>
-      <c r="C37" s="5" t="str">
+      <c r="C37" s="16" t="str">
         <f t="shared" si="1"/>
         <v>023</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="D37" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="10">
         <v>36</v>
       </c>
-      <c r="C38" s="5" t="str">
+      <c r="C38" s="11" t="str">
         <f t="shared" si="1"/>
         <v>024</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="D38" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="10">
         <v>37</v>
       </c>
-      <c r="C39" s="5" t="str">
+      <c r="C39" s="11" t="str">
         <f t="shared" si="1"/>
         <v>025</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="D39" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="10">
         <v>38</v>
       </c>
-      <c r="C40" s="5" t="str">
+      <c r="C40" s="11" t="str">
         <f t="shared" si="1"/>
         <v>026</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="D40" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="10">
         <v>39</v>
       </c>
-      <c r="C41" s="5" t="str">
+      <c r="C41" s="11" t="str">
         <f t="shared" si="1"/>
         <v>027</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>